<commit_message>
Modul Manage Pegawai : Pemisahan user jakarta dan cilacap, Modul Pengumuman dan Slip Gaji : Tambah Save as PDF, Modul Reminder : tambah send 3 email
</commit_message>
<xml_diff>
--- a/public/form/Detail Slip Gaji.xlsx
+++ b/public/form/Detail Slip Gaji.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\s2p-helper\s2p-helper\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/s2p-project/s2p-helper/public/form/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{264193D3-97AD-A142-BA75-8431857EE1D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11850"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="11860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -71,9 +72,6 @@
     <t>20220002J</t>
   </si>
   <si>
-    <t>NIK</t>
-  </si>
-  <si>
     <t>Pendapatan Lain 1</t>
   </si>
   <si>
@@ -129,12 +127,15 @@
   </si>
   <si>
     <t>Approver</t>
+  </si>
+  <si>
+    <t>NPK</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -544,34 +545,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E20" sqref="E20"/>
+      <selection pane="bottomRight" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" customWidth="1"/>
-    <col min="3" max="8" width="22.140625" customWidth="1"/>
-    <col min="9" max="13" width="17.28515625" customWidth="1"/>
+    <col min="1" max="1" width="16.5" customWidth="1"/>
+    <col min="2" max="2" width="17.5" customWidth="1"/>
+    <col min="3" max="8" width="22.1640625" customWidth="1"/>
+    <col min="9" max="13" width="17.33203125" customWidth="1"/>
     <col min="14" max="18" width="17" customWidth="1"/>
-    <col min="19" max="22" width="23.28515625" customWidth="1"/>
-    <col min="23" max="25" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="22" width="23.33203125" customWidth="1"/>
+    <col min="23" max="25" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="26" max="27" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>0</v>
@@ -607,51 +608,51 @@
         <v>10</v>
       </c>
       <c r="N1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="O1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>26</v>
-      </c>
-      <c r="P1" s="5" t="s">
-        <v>27</v>
       </c>
       <c r="Q1" s="5" t="s">
         <v>11</v>
       </c>
       <c r="R1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="S1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="T1" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="U1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="V1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="W1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="X1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z1" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="S1" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="T1" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="U1" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="V1" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="W1" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="X1" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="Y1" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="Z1" s="8" t="s">
+      <c r="AA1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="AA1" s="8" t="s">
-        <v>21</v>
-      </c>
     </row>
-    <row r="2" spans="1:27" s="10" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" s="10" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>13</v>
@@ -722,12 +723,12 @@
       <c r="Z2" s="9"/>
       <c r="AA2" s="9"/>
     </row>
-    <row r="3" spans="1:27" s="10" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" s="10" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C3" s="9">
         <v>100000</v>
@@ -795,9 +796,9 @@
       <c r="Z3" s="9"/>
       <c r="AA3" s="9"/>
     </row>
-    <row r="4" spans="1:27" s="10" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" s="10" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>14</v>
@@ -868,9 +869,9 @@
       <c r="Z4" s="9"/>
       <c r="AA4" s="9"/>
     </row>
-    <row r="5" spans="1:27" s="10" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" s="10" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>12</v>

</xml_diff>